<commit_message>
modify user controller update method
</commit_message>
<xml_diff>
--- a/public/download/sample/CM.xlsx
+++ b/public/download/sample/CM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20400" windowHeight="7530"/>
+    <workbookView windowWidth="14250" windowHeight="8115"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
   <si>
     <t>DD Code</t>
   </si>
@@ -49,7 +49,7 @@
     <t>Address</t>
   </si>
   <si>
-    <t>Joning Date</t>
+    <t>Joining Date</t>
   </si>
   <si>
     <t>Bank Account Name</t>
@@ -797,7 +797,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -813,17 +813,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="178" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="180" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1379,8 +1373,8 @@
   <sheetPr/>
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2:Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="33.1428571428571" defaultRowHeight="15" outlineLevelRow="4"/>
@@ -1449,13 +1443,13 @@
       <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="6" t="s">
         <v>16</v>
       </c>
       <c r="R1" s="3" t="s">
@@ -1475,16 +1469,16 @@
       <c r="D2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>1958041928</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="4">
         <v>1715969790</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="5">
         <v>30806</v>
       </c>
       <c r="I2" s="4" t="s">
@@ -1496,7 +1490,7 @@
       <c r="K2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="6">
+      <c r="L2" s="5">
         <v>41122</v>
       </c>
       <c r="M2" s="4" t="s">
@@ -1505,14 +1499,16 @@
       <c r="N2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="O2" s="9" t="s">
         <v>27</v>
       </c>
       <c r="P2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5">
+      <c r="Q2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R2" s="4">
         <v>15340</v>
       </c>
     </row>
@@ -1529,16 +1525,16 @@
       <c r="D3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>1958041927</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>1912345399</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="4">
         <v>6013465411</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="5">
         <v>36439</v>
       </c>
       <c r="I3" s="4" t="s">
@@ -1550,7 +1546,7 @@
       <c r="K3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L3" s="5">
         <v>44075</v>
       </c>
       <c r="M3" s="4" t="s">
@@ -1559,14 +1555,16 @@
       <c r="N3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="O3" s="9">
+      <c r="O3" s="7">
         <v>18582905628</v>
       </c>
       <c r="P3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5">
+      <c r="Q3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R3" s="4">
         <v>10200</v>
       </c>
     </row>
@@ -1583,16 +1581,16 @@
       <c r="D4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>1958025783</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>1915162211</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <v>30186</v>
       </c>
       <c r="I4" s="4" t="s">
@@ -1604,7 +1602,7 @@
       <c r="K4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="5">
         <v>44927</v>
       </c>
       <c r="M4" s="4" t="s">
@@ -1613,14 +1611,16 @@
       <c r="N4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="O4" s="9">
+      <c r="O4" s="7">
         <v>7017331933101</v>
       </c>
       <c r="P4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5">
+      <c r="Q4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R4" s="4">
         <v>9000</v>
       </c>
     </row>
@@ -1637,16 +1637,16 @@
       <c r="D5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>1958041930</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>1912317878</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <v>33675</v>
       </c>
       <c r="I5" s="4" t="s">
@@ -1658,7 +1658,7 @@
       <c r="K5" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L5" s="5">
         <v>42370</v>
       </c>
       <c r="M5" s="4" t="s">
@@ -1667,14 +1667,16 @@
       <c r="N5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="O5" s="9">
+      <c r="O5" s="7">
         <v>1731510105407</v>
       </c>
       <c r="P5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5">
+      <c r="Q5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R5" s="4">
         <v>10200</v>
       </c>
     </row>

</xml_diff>